<commit_message>
lecture multi page dans excel
</commit_message>
<xml_diff>
--- a/LecteurCatalogueFonction/data/validationMOA.xlsx
+++ b/LecteurCatalogueFonction/data/validationMOA.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="248">
   <si>
     <t>Espace</t>
   </si>
@@ -754,13 +755,25 @@
   </si>
   <si>
     <t>Voir F.Abrioux</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>auteur</t>
+  </si>
+  <si>
+    <t>le livre</t>
+  </si>
+  <si>
+    <t>fabien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1150,21 +1163,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -1176,7 +1189,7 @@
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1235,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1242,7 +1255,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1262,7 +1275,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1282,7 +1295,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1315,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1322,7 +1335,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1355,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1382,7 +1395,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1402,7 +1415,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1422,7 +1435,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1455,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1462,7 +1475,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1482,7 +1495,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1502,7 +1515,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1522,7 +1535,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1542,7 +1555,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +1575,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1582,7 +1595,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1602,7 +1615,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1622,7 +1635,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1642,7 +1655,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1662,7 +1675,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1682,7 +1695,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1702,7 +1715,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1722,7 +1735,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1742,7 +1755,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1765,7 +1778,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1785,7 +1798,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1825,7 +1838,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -1848,7 +1861,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1871,7 +1884,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1891,7 +1904,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1917,7 +1930,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -1937,7 +1950,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -1957,7 +1970,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -1977,7 +1990,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -1997,7 +2010,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -2017,7 +2030,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -2037,7 +2050,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -2057,7 +2070,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -2077,7 +2090,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -2097,7 +2110,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -2120,7 +2133,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2146,7 +2159,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>101</v>
       </c>
@@ -2166,7 +2179,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>101</v>
       </c>
@@ -2186,7 +2199,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -2206,7 +2219,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -2226,7 +2239,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -2246,7 +2259,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2266,7 +2279,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -2286,7 +2299,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -2306,7 +2319,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -2326,7 +2339,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -2346,7 +2359,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>101</v>
       </c>
@@ -2366,7 +2379,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -2386,7 +2399,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -2406,7 +2419,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -2426,7 +2439,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -2446,7 +2459,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>101</v>
       </c>
@@ -2466,7 +2479,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -2486,7 +2499,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -2506,7 +2519,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -2526,7 +2539,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -2546,7 +2559,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -2566,7 +2579,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -2586,7 +2599,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -2609,7 +2622,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>63</v>
       </c>
@@ -2632,7 +2645,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>101</v>
       </c>
@@ -2652,7 +2665,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>101</v>
       </c>
@@ -2672,7 +2685,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>101</v>
       </c>
@@ -2692,7 +2705,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>101</v>
       </c>
@@ -2712,7 +2725,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -2735,7 +2748,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -2758,7 +2771,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -2781,7 +2794,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -2804,7 +2817,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -2827,7 +2840,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -2850,7 +2863,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -2870,7 +2883,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>163</v>
       </c>
@@ -2893,7 +2906,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>159</v>
       </c>
@@ -2913,7 +2926,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>163</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>159</v>
       </c>
@@ -2962,7 +2975,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>63</v>
       </c>
@@ -2985,7 +2998,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>63</v>
       </c>
@@ -3008,7 +3021,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>159</v>
       </c>
@@ -3031,7 +3044,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>163</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>159</v>
       </c>
@@ -3083,7 +3096,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>159</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -3126,7 +3139,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>63</v>
       </c>
@@ -3149,7 +3162,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>63</v>
       </c>
@@ -3169,7 +3182,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -3189,7 +3202,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>63</v>
       </c>
@@ -3209,7 +3222,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>63</v>
       </c>
@@ -3229,7 +3242,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>63</v>
       </c>
@@ -3249,7 +3262,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>63</v>
       </c>
@@ -3269,7 +3282,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -3292,7 +3305,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>221</v>
       </c>
@@ -3312,7 +3325,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -3332,7 +3345,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -3352,7 +3365,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -3372,7 +3385,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>63</v>
       </c>
@@ -3405,4 +3418,35 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>